<commit_message>
updated reserved vaccines and new types
</commit_message>
<xml_diff>
--- a/data_vaccines_information.xlsx
+++ b/data_vaccines_information.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waj\OneDrive - AWK Group AG\80_prog\projects\petproject_impfcounter_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waj\OneDrive - AWK Group AG\80_prog\projects\petproject_impfcounter_data_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905FC65A-DBD8-4EB9-864B-D24DCDA24B17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BA99E9-D894-4C0F-BC58-6A4E03D54E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
+    <workbookView xWindow="708" yWindow="5676" windowWidth="12180" windowHeight="10752" xr2:uid="{AAC3A440-B87B-437D-9B31-8ABA125153B9}"/>
   </bookViews>
   <sheets>
     <sheet name="vaccines" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Wäfler, Jonas</author>
+  </authors>
+  <commentList>
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{C3ECA0AE-901C-44F3-A1F2-26B4C98295AF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Wäfler, Jonas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+2. agreement 3.2.2021: additional 6M (total 
+13.5)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="93">
   <si>
     <t>manufacturer</t>
   </si>
@@ -271,6 +306,48 @@
   </si>
   <si>
     <t>Next-generation vaccine platforms for COVID-19 (english)</t>
+  </si>
+  <si>
+    <t>Curevac</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>Novavax</t>
+  </si>
+  <si>
+    <t>not approved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wikipedia: </t>
+  </si>
+  <si>
+    <t>COVID-19 vaccine</t>
+  </si>
+  <si>
+    <t>SARS-CoV-2-Impfstoff</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/SARS-CoV-2-Impfstoff</t>
+  </si>
+  <si>
+    <t>https://de.wikipedia.org/wiki/CVnCoV</t>
+  </si>
+  <si>
+    <t>Zorecimeran</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>NVX-CoV2373</t>
+  </si>
+  <si>
+    <t>recombinant nanoparticle vaccine</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Novavax_COVID-19_vaccine</t>
   </si>
 </sst>
 </file>
@@ -281,7 +358,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -306,6 +383,19 @@
       <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -378,6 +468,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -676,19 +770,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9A27E4-6C71-419D-AA20-A71F9176CE9B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9A27E4-6C71-419D-AA20-A71F9176CE9B}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="47.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
     <col min="8" max="8" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="14.77734375" customWidth="1"/>
@@ -832,7 +927,7 @@
         <v>44208</v>
       </c>
       <c r="N3" s="5">
-        <v>7500000</v>
+        <v>13500000</v>
       </c>
       <c r="O3" s="8">
         <v>44050</v>
@@ -865,7 +960,7 @@
         <v>44</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="K4" t="s">
         <v>45</v>
@@ -890,7 +985,7 @@
       <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>54</v>
       </c>
       <c r="D5" t="s">
@@ -910,10 +1005,10 @@
         <v>13</v>
       </c>
       <c r="J5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="K5" t="s">
-        <v>34</v>
       </c>
       <c r="L5" t="s">
         <v>32</v>
@@ -927,25 +1022,113 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="7">
+        <v>2</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="5">
+        <v>5000000</v>
+      </c>
+      <c r="O6" s="8">
+        <v>44230</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="5">
+        <v>6000000</v>
+      </c>
+      <c r="O7" s="8">
+        <v>44230</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{98DB1DBA-983E-42CE-8F54-2C4B79A18A29}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{4C48AC4A-28EC-4CAD-ABDF-D14CCDC5B03A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6ECE3-E724-45D0-9B6A-D4576F16769D}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1054,15 +1237,45 @@
         <v>56</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{1805E364-CC7E-4892-B2A6-9BC08A7DE88D}"/>
+    <hyperlink ref="D8" r:id="rId2" xr:uid="{13AC84F9-A2C9-4F33-B57B-C86D93C826C1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001CF2E9C31C1F9249AD1C5C32C883CF52" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2446087b74f13e01ab9e6ca0cc8aa566">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f809d0f6-fdde-443e-9ae6-18ec6b857c37" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04f7e70fe4e704e7e2502280d2be185a" ns3:_="">
     <xsd:import namespace="f809d0f6-fdde-443e-9ae6-18ec6b857c37"/>
@@ -1240,22 +1453,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44E5A0E9-E8A9-4737-9AA5-8E5511C32371}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1271,21 +1486,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2919F63-2E5A-4F33-AAD9-737AEBDDF6E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E59A23A-D64F-4C65-B820-448A798A73C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>